<commit_message>
docs: 📝 update docs
</commit_message>
<xml_diff>
--- a/es/es-adj.xlsx
+++ b/es/es-adj.xlsx
@@ -32,363 +32,384 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="145">
   <si>
     <t>Spanish</t>
   </si>
   <si>
+    <t>French</t>
+  </si>
+  <si>
+    <t>negro</t>
+  </si>
+  <si>
+    <t>noir</t>
+  </si>
+  <si>
+    <t>blanco</t>
+  </si>
+  <si>
+    <t>blanc</t>
+  </si>
+  <si>
+    <t>gris</t>
+  </si>
+  <si>
+    <t>marrón</t>
+  </si>
+  <si>
+    <t>brun</t>
+  </si>
+  <si>
+    <t>azul</t>
+  </si>
+  <si>
+    <t>bleu</t>
+  </si>
+  <si>
+    <t>verde</t>
+  </si>
+  <si>
+    <t>vert</t>
+  </si>
+  <si>
+    <t>rojo</t>
+  </si>
+  <si>
+    <t>rouge</t>
+  </si>
+  <si>
+    <t>rosa</t>
+  </si>
+  <si>
+    <t>rose</t>
+  </si>
+  <si>
+    <t>amarillo</t>
+  </si>
+  <si>
+    <t>jaune</t>
+  </si>
+  <si>
+    <t>naranja</t>
+  </si>
+  <si>
+    <t>orange</t>
+  </si>
+  <si>
+    <t>púrpura</t>
+  </si>
+  <si>
+    <t>violet</t>
+  </si>
+  <si>
+    <t>hermoso</t>
+  </si>
+  <si>
+    <t>beau</t>
+  </si>
+  <si>
+    <t>feo</t>
+  </si>
+  <si>
+    <t>laid</t>
+  </si>
+  <si>
+    <t>grande</t>
+  </si>
+  <si>
+    <t>grand</t>
+  </si>
+  <si>
+    <t>corto</t>
+  </si>
+  <si>
+    <t>court</t>
+  </si>
+  <si>
+    <t>antiguo</t>
+  </si>
+  <si>
+    <t>ancien</t>
+  </si>
+  <si>
+    <t>joven</t>
+  </si>
+  <si>
+    <t>jeune</t>
+  </si>
+  <si>
+    <t>inteligente</t>
+  </si>
+  <si>
+    <t>intelligent</t>
+  </si>
+  <si>
+    <t>estúpido</t>
+  </si>
+  <si>
+    <t>stupide</t>
+  </si>
+  <si>
+    <t>bucle</t>
+  </si>
+  <si>
+    <t>bouclé</t>
+  </si>
+  <si>
+    <t>bien</t>
+  </si>
+  <si>
+    <t>droit</t>
+  </si>
+  <si>
+    <t>fuerte</t>
+  </si>
+  <si>
+    <t>fort</t>
+  </si>
+  <si>
+    <t>débil</t>
+  </si>
+  <si>
+    <t>faible</t>
+  </si>
+  <si>
+    <t>rico</t>
+  </si>
+  <si>
+    <t>riche</t>
+  </si>
+  <si>
+    <t>pobre</t>
+  </si>
+  <si>
+    <t>pauvre</t>
+  </si>
+  <si>
+    <t>alemán</t>
+  </si>
+  <si>
+    <t>allemand</t>
+  </si>
+  <si>
+    <t>camboyano</t>
+  </si>
+  <si>
+    <t>cambodgien</t>
+  </si>
+  <si>
+    <t>austriaco</t>
+  </si>
+  <si>
+    <t>autrichien</t>
+  </si>
+  <si>
+    <t>coreano</t>
+  </si>
+  <si>
+    <t>coréen</t>
+  </si>
+  <si>
+    <t>holandés</t>
+  </si>
+  <si>
+    <t>néelandais</t>
+  </si>
+  <si>
+    <t>griego</t>
+  </si>
+  <si>
+    <t>grec</t>
+  </si>
+  <si>
+    <t>danés</t>
+  </si>
+  <si>
+    <t>danois</t>
+  </si>
+  <si>
+    <t>sueco</t>
+  </si>
+  <si>
+    <t>suédois</t>
+  </si>
+  <si>
+    <t>turco</t>
+  </si>
+  <si>
+    <t>turc</t>
+  </si>
+  <si>
+    <t>pequeño</t>
+  </si>
+  <si>
+    <t>petit</t>
+  </si>
+  <si>
+    <t>lleno</t>
+  </si>
+  <si>
+    <t>plein</t>
+  </si>
+  <si>
+    <t>vacío</t>
+  </si>
+  <si>
+    <t>vide</t>
+  </si>
+  <si>
+    <t>largo</t>
+  </si>
+  <si>
+    <t>long</t>
+  </si>
+  <si>
+    <t>propio</t>
+  </si>
+  <si>
+    <t>propre</t>
+  </si>
+  <si>
+    <t>sucio</t>
+  </si>
+  <si>
+    <t>sale</t>
+  </si>
+  <si>
+    <t>grueso</t>
+  </si>
+  <si>
+    <t>épais</t>
+  </si>
+  <si>
+    <t>esbelto</t>
+  </si>
+  <si>
+    <t>svelte</t>
+  </si>
+  <si>
+    <t>ancho</t>
+  </si>
+  <si>
+    <t>large</t>
+  </si>
+  <si>
+    <t>angosto</t>
+  </si>
+  <si>
+    <t>étroit</t>
+  </si>
+  <si>
+    <t>pesado</t>
+  </si>
+  <si>
+    <t>lourd</t>
+  </si>
+  <si>
+    <t>ligero</t>
+  </si>
+  <si>
+    <t>léger</t>
+  </si>
+  <si>
+    <t>azúcar</t>
+  </si>
+  <si>
+    <t>sucre</t>
+  </si>
+  <si>
+    <t>ácido</t>
+  </si>
+  <si>
+    <t>acide</t>
+  </si>
+  <si>
+    <t>oscuro</t>
+  </si>
+  <si>
+    <t>sombre</t>
+  </si>
+  <si>
+    <t>claro</t>
+  </si>
+  <si>
+    <t>alto</t>
+  </si>
+  <si>
+    <t>haut</t>
+  </si>
+  <si>
+    <t>abajo</t>
+  </si>
+  <si>
+    <t>bas</t>
+  </si>
+  <si>
+    <t>seco</t>
+  </si>
+  <si>
+    <t>sec</t>
+  </si>
+  <si>
+    <t>húmedo</t>
+  </si>
+  <si>
+    <t>humide</t>
+  </si>
+  <si>
+    <t>nuevo</t>
+  </si>
+  <si>
+    <t>nouveau</t>
+  </si>
+  <si>
+    <t>viejo</t>
+  </si>
+  <si>
+    <t>vieux</t>
+  </si>
+  <si>
+    <t>frío</t>
+  </si>
+  <si>
+    <t>froid</t>
+  </si>
+  <si>
+    <t>caliente</t>
+  </si>
+  <si>
+    <t>chaud</t>
+  </si>
+  <si>
+    <t>idéntico</t>
+  </si>
+  <si>
+    <t>identique</t>
+  </si>
+  <si>
+    <t>diferente</t>
+  </si>
+  <si>
+    <t>différent</t>
+  </si>
+  <si>
     <t>English</t>
   </si>
   <si>
-    <t>negro</t>
-  </si>
-  <si>
-    <t>black</t>
-  </si>
-  <si>
-    <t>blanco</t>
-  </si>
-  <si>
-    <t>white</t>
-  </si>
-  <si>
-    <t>gris</t>
-  </si>
-  <si>
-    <t>gray</t>
-  </si>
-  <si>
-    <t>marrón</t>
-  </si>
-  <si>
-    <t>brown</t>
-  </si>
-  <si>
-    <t>azul</t>
-  </si>
-  <si>
-    <t>blue</t>
-  </si>
-  <si>
-    <t>verde</t>
-  </si>
-  <si>
-    <t>green</t>
-  </si>
-  <si>
-    <t>rojo</t>
-  </si>
-  <si>
-    <t>red</t>
-  </si>
-  <si>
-    <t>rosa</t>
-  </si>
-  <si>
-    <t>pink</t>
-  </si>
-  <si>
-    <t>amarillo</t>
-  </si>
-  <si>
-    <t>yellow</t>
-  </si>
-  <si>
-    <t>naranja</t>
-  </si>
-  <si>
-    <t>orange</t>
-  </si>
-  <si>
-    <t>púrpura</t>
-  </si>
-  <si>
-    <t>purple</t>
-  </si>
-  <si>
-    <t>hermoso</t>
-  </si>
-  <si>
-    <t>beautiful</t>
-  </si>
-  <si>
-    <t>feo</t>
-  </si>
-  <si>
-    <t>ugly</t>
-  </si>
-  <si>
-    <t>grande</t>
-  </si>
-  <si>
-    <t>tall</t>
-  </si>
-  <si>
-    <t>corto</t>
-  </si>
-  <si>
-    <t>short</t>
-  </si>
-  <si>
-    <t>antiguo</t>
-  </si>
-  <si>
-    <t>old</t>
-  </si>
-  <si>
-    <t>joven</t>
-  </si>
-  <si>
-    <t>young</t>
-  </si>
-  <si>
-    <t>inteligente</t>
-  </si>
-  <si>
-    <t>estúpido</t>
-  </si>
-  <si>
-    <t>bucle</t>
-  </si>
-  <si>
-    <t>curly</t>
-  </si>
-  <si>
-    <t>bien</t>
-  </si>
-  <si>
-    <t>straight</t>
-  </si>
-  <si>
-    <t>fuerte</t>
-  </si>
-  <si>
-    <t>débil</t>
-  </si>
-  <si>
-    <t>rico</t>
-  </si>
-  <si>
-    <t>pobre</t>
-  </si>
-  <si>
-    <t>alemán</t>
-  </si>
-  <si>
-    <t>German</t>
-  </si>
-  <si>
-    <t>camboyano</t>
-  </si>
-  <si>
-    <t>Cambodian</t>
-  </si>
-  <si>
-    <t>austriaco</t>
-  </si>
-  <si>
-    <t>Austrian</t>
-  </si>
-  <si>
-    <t>coreano</t>
-  </si>
-  <si>
-    <t>Korean</t>
-  </si>
-  <si>
-    <t>holandés</t>
-  </si>
-  <si>
-    <t>Dutch</t>
-  </si>
-  <si>
-    <t>griego</t>
-  </si>
-  <si>
-    <t>Greek</t>
-  </si>
-  <si>
-    <t>danés</t>
-  </si>
-  <si>
-    <t>Danish</t>
-  </si>
-  <si>
-    <t>sueco</t>
-  </si>
-  <si>
-    <t>Swedish</t>
-  </si>
-  <si>
-    <t>turco</t>
-  </si>
-  <si>
-    <t>Turkish</t>
-  </si>
-  <si>
-    <t>big</t>
-  </si>
-  <si>
-    <t>pequeño</t>
-  </si>
-  <si>
-    <t>small</t>
-  </si>
-  <si>
-    <t>lleno</t>
-  </si>
-  <si>
-    <t>full</t>
-  </si>
-  <si>
-    <t>vacío</t>
-  </si>
-  <si>
-    <t>empty</t>
-  </si>
-  <si>
-    <t>largo</t>
-  </si>
-  <si>
-    <t>long</t>
-  </si>
-  <si>
-    <t>propio</t>
-  </si>
-  <si>
-    <t>clean</t>
-  </si>
-  <si>
-    <t>sucio</t>
-  </si>
-  <si>
-    <t>dirty</t>
-  </si>
-  <si>
-    <t>grueso</t>
-  </si>
-  <si>
-    <t>thick</t>
-  </si>
-  <si>
-    <t>esbelto</t>
-  </si>
-  <si>
-    <t>slim</t>
-  </si>
-  <si>
-    <t>ancho</t>
-  </si>
-  <si>
-    <t>wide</t>
-  </si>
-  <si>
-    <t>angosto</t>
-  </si>
-  <si>
-    <t>narrow</t>
-  </si>
-  <si>
-    <t>pesado</t>
-  </si>
-  <si>
-    <t>heavy</t>
-  </si>
-  <si>
-    <t>ligero</t>
-  </si>
-  <si>
-    <t>light</t>
-  </si>
-  <si>
-    <t>azúcar</t>
-  </si>
-  <si>
-    <t>sweet</t>
-  </si>
-  <si>
-    <t>ácido</t>
-  </si>
-  <si>
-    <t>sour</t>
-  </si>
-  <si>
-    <t>oscuro</t>
-  </si>
-  <si>
-    <t>dark</t>
-  </si>
-  <si>
-    <t>claro</t>
-  </si>
-  <si>
-    <t>alto</t>
-  </si>
-  <si>
-    <t>high</t>
-  </si>
-  <si>
-    <t>abajo</t>
-  </si>
-  <si>
-    <t>low</t>
-  </si>
-  <si>
-    <t>seco</t>
-  </si>
-  <si>
-    <t>dry</t>
-  </si>
-  <si>
-    <t>húmedo</t>
-  </si>
-  <si>
-    <t>wet</t>
-  </si>
-  <si>
-    <t>nueve</t>
-  </si>
-  <si>
-    <t>new</t>
-  </si>
-  <si>
-    <t>viejo</t>
-  </si>
-  <si>
-    <t>frío</t>
-  </si>
-  <si>
-    <t>cold</t>
-  </si>
-  <si>
-    <t>caliente</t>
-  </si>
-  <si>
-    <t>hot</t>
-  </si>
-  <si>
-    <t>idéntico</t>
-  </si>
-  <si>
-    <t>same</t>
-  </si>
-  <si>
-    <t>diferente</t>
-  </si>
-  <si>
-    <t>different</t>
-  </si>
-  <si>
     <t>encantado</t>
   </si>
   <si>
+    <t>content</t>
+  </si>
+  <si>
     <t>triste</t>
   </si>
   <si>
-    <t>good</t>
-  </si>
-  <si>
-    <t>malo</t>
+    <t>bon</t>
+  </si>
+  <si>
+    <t>mauvais</t>
   </si>
   <si>
     <t>bad</t>
@@ -397,46 +418,55 @@
     <t>mejor</t>
   </si>
   <si>
-    <t>better</t>
-  </si>
-  <si>
-    <t>peor</t>
+    <t>mal</t>
   </si>
   <si>
     <t>worse</t>
   </si>
   <si>
+    <t>meilleur</t>
+  </si>
+  <si>
+    <t>pire</t>
+  </si>
+  <si>
+    <t>pis</t>
+  </si>
+  <si>
     <t>siempre</t>
   </si>
   <si>
-    <t>always</t>
+    <t>toujours</t>
   </si>
   <si>
     <t>alrededor</t>
   </si>
   <si>
+    <t>autour</t>
+  </si>
+  <si>
     <t>a menudo</t>
   </si>
   <si>
-    <t>often</t>
+    <t>souvent</t>
   </si>
   <si>
     <t>a veces</t>
   </si>
   <si>
-    <t>sometimes</t>
+    <t>parfois</t>
   </si>
   <si>
     <t>casi nunca</t>
   </si>
   <si>
-    <t>rarely</t>
+    <t>rarement</t>
   </si>
   <si>
     <t>nunca</t>
   </si>
   <si>
-    <t>never</t>
+    <t>jamais</t>
   </si>
 </sst>
 </file>
@@ -1611,7 +1641,7 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView zoomScale="151" zoomScaleNormal="151" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="D1" sqref="D1:D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8" outlineLevelRow="6" outlineLevelCol="3"/>
@@ -1649,63 +1679,63 @@
         <v>6</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="D3" s="2" t="s">
         <v>8</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="C4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="D4" s="2" t="s">
         <v>12</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="C5" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="D5" s="2" t="s">
         <v>16</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="C6" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="D6" s="2" t="s">
         <v>20</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>22</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>23</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
@@ -1722,7 +1752,7 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView zoomScale="156" zoomScaleNormal="156" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8" outlineLevelCol="3"/>
@@ -1746,89 +1776,101 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="C3" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="D3" s="2" t="s">
         <v>30</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="C4" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="D4" s="2" t="s">
         <v>34</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B5" s="1"/>
       <c r="C5" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="D5" s="1"/>
+      <c r="D5" s="1" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B7" s="1"/>
+        <v>43</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>44</v>
+      </c>
       <c r="C7" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="D7" s="1"/>
+        <v>45</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B8" s="1"/>
+        <v>47</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>48</v>
+      </c>
       <c r="C8" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="D8" s="1"/>
+        <v>49</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="1"/>
@@ -1848,7 +1890,7 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8" outlineLevelRow="7" outlineLevelCol="3"/>
@@ -1875,74 +1917,74 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="1" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="1" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="1" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -1963,7 +2005,7 @@
   <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView zoomScale="172" zoomScaleNormal="172" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:G8"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8" outlineLevelCol="7"/>
@@ -1996,184 +2038,184 @@
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>64</v>
-      </c>
       <c r="C2" s="2" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="2" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="C3" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>31</v>
-      </c>
       <c r="E3" s="2" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="2" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="2" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="2" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="2" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>33</v>
+        <v>111</v>
       </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="2" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>109</v>
+        <v>114</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
     </row>
     <row r="9" spans="5:8">
@@ -2194,7 +2236,7 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8" outlineLevelCol="3"/>
@@ -2207,58 +2249,70 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>0</v>
-      </c>
       <c r="D1" s="2" t="s">
-        <v>1</v>
+        <v>120</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="1" t="s">
-        <v>115</v>
+        <v>121</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
+        <v>122</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>123</v>
+      </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>117</v>
+        <v>124</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>118</v>
+        <v>125</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>119</v>
+        <v>126</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>121</v>
-      </c>
+        <v>127</v>
+      </c>
+      <c r="B4"/>
       <c r="C4" s="1" t="s">
-        <v>122</v>
+        <v>128</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>123</v>
+        <v>129</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
+      <c r="B5" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>131</v>
+      </c>
       <c r="D5" s="4"/>
+    </row>
+    <row r="6" spans="2:3">
+      <c r="B6" s="1"/>
+      <c r="C6" s="1" t="s">
+        <v>132</v>
+      </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="1"/>
@@ -2290,7 +2344,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="173" zoomScaleNormal="173" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="D1" sqref="D1:D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8" outlineLevelRow="5" outlineLevelCol="3"/>
@@ -2315,52 +2369,54 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>125</v>
+        <v>133</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>134</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="D2" s="1"/>
+        <v>135</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>136</v>
+      </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="1" t="s">
-        <v>127</v>
+        <v>137</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>128</v>
+        <v>138</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="1" t="s">
-        <v>129</v>
+        <v>139</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>130</v>
+        <v>140</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="1" t="s">
-        <v>131</v>
+        <v>141</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>132</v>
+        <v>142</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="1" t="s">
-        <v>133</v>
+        <v>143</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>134</v>
+        <v>144</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>

</xml_diff>